<commit_message>
planilhado desconsiderando planilhas já geradas
</commit_message>
<xml_diff>
--- a/estimativa/modelo.xlsx
+++ b/estimativa/modelo.xlsx
@@ -518,6 +518,96 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -538,96 +628,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -976,37 +976,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:D27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
@@ -1049,32 +1049,32 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="34"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="64"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1"/>
@@ -1106,13 +1106,13 @@
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1126,29 +1126,29 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="11"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="11"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1"/>
@@ -1177,12 +1177,12 @@
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
       <c r="E15" s="13" t="s">
         <v>14</v>
       </c>
@@ -1190,33 +1190,33 @@
         <v>9</v>
       </c>
       <c r="G15" s="15"/>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="45"/>
-      <c r="J15" s="37"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="36" t="s">
+      <c r="H16" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="37"/>
+      <c r="I16" s="51"/>
       <c r="J16" s="16">
-        <v>1.1499999999999999</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="15"/>
@@ -1225,48 +1225,48 @@
       <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="44" t="s">
+      <c r="H18" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="37"/>
+      <c r="I19" s="51"/>
       <c r="J19" s="16"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="43" t="s">
+    <row r="20" spans="1:10" ht="27" customHeight="1">
+      <c r="A20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1"/>
@@ -1295,80 +1295,80 @@
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="20"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41"/>
       <c r="G24" s="20"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="50" t="s">
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
     </row>
     <row r="26" spans="1:10" ht="16.5">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38" t="s">
+      <c r="B26" s="42"/>
+      <c r="C26" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="50" t="s">
+      <c r="D26" s="42"/>
+      <c r="E26" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50" t="s">
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1"/>
@@ -1396,19 +1396,19 @@
       <c r="I29" s="23"/>
       <c r="J29" s="23"/>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="53" t="s">
+    <row r="30" spans="1:10" ht="30.75" customHeight="1">
+      <c r="A30" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="55"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="48"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1"/>
@@ -1437,54 +1437,54 @@
       <c r="J32" s="23"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
       <c r="F33" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="58"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
       <c r="F34" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="59"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="58"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="30"/>
       <c r="F35" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="59"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="59"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="26"/>
@@ -1499,29 +1499,42 @@
       <c r="J36" s="26"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="60" t="s">
+      <c r="A37" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="60"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="62" t="s">
+      <c r="B37" s="32"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="64"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="H18:J18"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="G33:J33"/>
     <mergeCell ref="A20:J20"/>
@@ -1538,25 +1551,12 @@
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="H27:J27"/>
     <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:J37"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>